<commit_message>
Removes capacity construction and dist solar levers
</commit_message>
<xml_diff>
--- a/InputData/elec/GHESS/Green Hydrogen Electricity Supply Shareweights.xlsx
+++ b/InputData/elec/GHESS/Green Hydrogen Electricity Supply Shareweights.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\TTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\elec\GHESS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460419F9-E16A-400F-91E6-BD5553EB796E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625088B9-66B7-410C-A5F8-26D776B79511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31260" yWindow="660" windowWidth="21600" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Max Fraction of Production (dimensionless)</t>
   </si>
@@ -109,9 +109,6 @@
     <t>hydrogen combined cycle</t>
   </si>
   <si>
-    <t>Source: None Needed</t>
-  </si>
-  <si>
     <t>Notes:</t>
   </si>
   <si>
@@ -134,6 +131,27 @@
   </si>
   <si>
     <t>GHESS Green Hydrogen Electricity Supply Shareweights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clean Hydrogen Monitor 2022 report. </t>
+  </si>
+  <si>
+    <t>Source:</t>
+  </si>
+  <si>
+    <t>Electricity source for hydrogen projects</t>
+  </si>
+  <si>
+    <t>Hydrogen Europe</t>
+  </si>
+  <si>
+    <t>Clean Hydrogen Monitor 2022</t>
+  </si>
+  <si>
+    <t>https://hydrogeneurope.eu/wp-content/uploads/2022/10/Clean_Hydrogen_Monitor_10-2022_DIGITAL.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For the EU model, we calibrate these values to Hydrogen Europe's </t>
   </si>
 </sst>
 </file>
@@ -383,7 +401,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -563,6 +581,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -716,7 +740,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyProtection="0">
@@ -812,8 +836,9 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -822,8 +847,13 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="85"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="86">
     <cellStyle name="20% - Accent1" xfId="25" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="29" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="33" builtinId="38" customBuiltin="1"/>
@@ -865,6 +895,7 @@
     <cellStyle name="Heading 2" xfId="10" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="11" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="12" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="77" xr:uid="{E283E47E-2F86-4A89-8D02-E2992DD3D2DE}"/>
     <cellStyle name="Hyperlink 2 2" xfId="84" xr:uid="{2D4E116A-493D-4045-B7BA-CEF4D3AE7A96}"/>
     <cellStyle name="Hyperlink 3" xfId="74" xr:uid="{912A9BAB-AD28-435A-B4EA-160F8BFE9A24}"/>
@@ -1210,66 +1241,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="61.5703125" customWidth="1"/>
+    <col min="2" max="2" width="61.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
+      <c r="B5" s="6">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{310E439B-DF60-481D-B7B4-96DFF6CEEFA8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1281,15 +1354,15 @@
   <dimension ref="A1:AE25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B7" sqref="B7:AE7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1384,7 +1457,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1479,7 +1552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1574,7 +1647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1669,7 +1742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1764,7 +1837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1859,197 +1932,197 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="K7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="N7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="O7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="P7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="Q7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="R7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="S7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="T7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="U7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="V7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="W7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="X7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="Y7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="Z7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="AA7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="AB7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="AC7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="AD7">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="AE7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="N8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="O8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="P8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="Q8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="R8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="S8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="T8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="U8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="V8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="W8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="X8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="Y8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="Z8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AA8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AB8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AC8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AD8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AE8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2144,7 +2217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2239,7 +2312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2334,7 +2407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2429,7 +2502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2524,7 +2597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2619,102 +2692,102 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="J15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="K15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="L15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="M15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="N15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="O15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="P15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="Q15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="R15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="S15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="T15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="U15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="V15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="W15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="X15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="Y15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="Z15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AA15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AB15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AC15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AD15">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="AE15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -2809,7 +2882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -2904,7 +2977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -2999,7 +3072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -3094,7 +3167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -3189,7 +3262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -3284,7 +3357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -3379,7 +3452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -3474,7 +3547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -3569,7 +3642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>

</xml_diff>